<commit_message>
Moved ExcelReader class from pageObjects to Utilities package
Moved ExcelReader class from pageObjects to Utilities package
</commit_message>
<xml_diff>
--- a/Team12TechSquad/src/test/resources/Data/IngredientsAndComorbidities-ScrapperHackathon.xlsx
+++ b/Team12TechSquad/src/test/resources/Data/IngredientsAndComorbidities-ScrapperHackathon.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyProject\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dilin\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774680E7-38AB-43EC-BFEE-ADFD798D4A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6E3005-D8C1-4003-A0B1-F3068142B4EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final list for LFV Elimination " sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="250">
   <si>
     <t xml:space="preserve">Meal plan for Low Fat Vegan diet </t>
   </si>
@@ -567,6 +567,9 @@
   </si>
   <si>
     <t>flax seed</t>
+  </si>
+  <si>
+    <t>Meal plan for Low Carbohydrates High Fat (Keto) -LCHF</t>
   </si>
   <si>
     <t>Food Processing</t>
@@ -1178,7 +1181,7 @@
   </sheetPr>
   <dimension ref="A1:J90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
@@ -1322,7 +1325,7 @@
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="13">
+    <row r="10" spans="1:8">
       <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
@@ -1333,7 +1336,7 @@
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="13">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>34</v>
       </c>
@@ -2201,10 +2204,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15" customHeight="1"/>
@@ -2216,201 +2219,199 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
+        <v>180</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" customHeight="1">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" customHeight="1">
-      <c r="A2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>181</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15" customHeight="1">
       <c r="A3" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>184</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="8" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" customHeight="1">
       <c r="A4" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>187</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="8" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15" customHeight="1">
       <c r="A5" s="2" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>44</v>
+        <v>188</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15" customHeight="1">
       <c r="A6" s="2" t="s">
-        <v>26</v>
+        <v>190</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>191</v>
+        <v>44</v>
       </c>
       <c r="C6" s="2"/>
       <c r="D6" s="8" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" customHeight="1">
       <c r="A7" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>195</v>
+        <v>37</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="8" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>196</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C9" s="2"/>
+      <c r="D9" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
     </row>
     <row r="10" spans="1:4" ht="15" customHeight="1">
       <c r="A10" s="2" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>199</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
     </row>
     <row r="11" spans="1:4" ht="15" customHeight="1">
       <c r="A11" s="2" t="s">
-        <v>199</v>
+        <v>39</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
     <row r="12" spans="1:4" ht="15" customHeight="1">
       <c r="A12" s="2" t="s">
-        <v>49</v>
+        <v>200</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>200</v>
+        <v>13</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" spans="1:4" ht="15" customHeight="1">
       <c r="A13" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="15" customHeight="1">
       <c r="A14" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="15" customHeight="1">
       <c r="A15" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>206</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="15" customHeight="1">
       <c r="A16" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>208</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="15" customHeight="1">
       <c r="A17" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="B17" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>210</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="15" customHeight="1">
       <c r="A18" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>211</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>165</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -2420,27 +2421,27 @@
         <v>212</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="12.5">
+    <row r="20" spans="1:4" ht="15" customHeight="1">
       <c r="A20" s="2" t="s">
-        <v>31</v>
+        <v>213</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" ht="12.5">
       <c r="A21" s="2" t="s">
-        <v>213</v>
+        <v>31</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -2450,7 +2451,7 @@
         <v>214</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -2460,7 +2461,7 @@
         <v>215</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -2470,7 +2471,7 @@
         <v>216</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -2480,7 +2481,7 @@
         <v>217</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -2490,7 +2491,7 @@
         <v>218</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -2500,17 +2501,17 @@
         <v>219</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>220</v>
+        <v>175</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
     <row r="28" spans="1:4" ht="12.5">
       <c r="A28" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -2520,7 +2521,7 @@
         <v>222</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -2530,7 +2531,7 @@
         <v>223</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -2540,36 +2541,38 @@
         <v>224</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>225</v>
+        <v>179</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" spans="1:4" ht="12.5">
       <c r="A32" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>227</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" spans="1:4" ht="12.5">
       <c r="A33" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>228</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>229</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" ht="12.5">
       <c r="A34" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
@@ -2607,7 +2610,7 @@
     </row>
     <row r="39" spans="1:4" ht="12.5">
       <c r="A39" s="2" t="s">
-        <v>143</v>
+        <v>235</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -2615,7 +2618,7 @@
     </row>
     <row r="40" spans="1:4" ht="12.5">
       <c r="A40" s="2" t="s">
-        <v>137</v>
+        <v>143</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -2623,7 +2626,7 @@
     </row>
     <row r="41" spans="1:4" ht="12.5">
       <c r="A41" s="2" t="s">
-        <v>235</v>
+        <v>137</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -2647,7 +2650,7 @@
     </row>
     <row r="44" spans="1:4" ht="12.5">
       <c r="A44" s="2" t="s">
-        <v>75</v>
+        <v>238</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -2655,7 +2658,7 @@
     </row>
     <row r="45" spans="1:4" ht="12.5">
       <c r="A45" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -2663,7 +2666,7 @@
     </row>
     <row r="46" spans="1:4" ht="12.5">
       <c r="A46" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -2671,7 +2674,7 @@
     </row>
     <row r="47" spans="1:4" ht="12.5">
       <c r="A47" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -2679,7 +2682,7 @@
     </row>
     <row r="48" spans="1:4" ht="12.5">
       <c r="A48" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -2687,7 +2690,7 @@
     </row>
     <row r="49" spans="1:4" ht="12.5">
       <c r="A49" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2695,7 +2698,7 @@
     </row>
     <row r="50" spans="1:4" ht="12.5">
       <c r="A50" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -2703,7 +2706,7 @@
     </row>
     <row r="51" spans="1:4" ht="12.5">
       <c r="A51" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -2711,7 +2714,7 @@
     </row>
     <row r="52" spans="1:4" ht="12.5">
       <c r="A52" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -2719,7 +2722,7 @@
     </row>
     <row r="53" spans="1:4" ht="12.5">
       <c r="A53" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -2727,7 +2730,7 @@
     </row>
     <row r="54" spans="1:4" ht="12.5">
       <c r="A54" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -2735,7 +2738,7 @@
     </row>
     <row r="55" spans="1:4" ht="12.5">
       <c r="A55" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -2743,7 +2746,7 @@
     </row>
     <row r="56" spans="1:4" ht="12.5">
       <c r="A56" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -2751,7 +2754,7 @@
     </row>
     <row r="57" spans="1:4" ht="12.5">
       <c r="A57" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -2759,7 +2762,7 @@
     </row>
     <row r="58" spans="1:4" ht="12.5">
       <c r="A58" s="2" t="s">
-        <v>51</v>
+        <v>103</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -2767,7 +2770,7 @@
     </row>
     <row r="59" spans="1:4" ht="12.5">
       <c r="A59" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -2775,7 +2778,7 @@
     </row>
     <row r="60" spans="1:4" ht="12.5">
       <c r="A60" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2783,7 +2786,7 @@
     </row>
     <row r="61" spans="1:4" ht="12.5">
       <c r="A61" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -2791,7 +2794,7 @@
     </row>
     <row r="62" spans="1:4" ht="12.5">
       <c r="A62" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -2799,7 +2802,7 @@
     </row>
     <row r="63" spans="1:4" ht="12.5">
       <c r="A63" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -2807,7 +2810,7 @@
     </row>
     <row r="64" spans="1:4" ht="12.5">
       <c r="A64" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -2815,7 +2818,7 @@
     </row>
     <row r="65" spans="1:4" ht="12.5">
       <c r="A65" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -2823,7 +2826,7 @@
     </row>
     <row r="66" spans="1:4" ht="12.5">
       <c r="A66" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -2831,7 +2834,7 @@
     </row>
     <row r="67" spans="1:4" ht="12.5">
       <c r="A67" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -2839,7 +2842,7 @@
     </row>
     <row r="68" spans="1:4" ht="12.5">
       <c r="A68" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -2847,7 +2850,7 @@
     </row>
     <row r="69" spans="1:4" ht="12.5">
       <c r="A69" s="2" t="s">
-        <v>126</v>
+        <v>70</v>
       </c>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -2855,7 +2858,7 @@
     </row>
     <row r="70" spans="1:4" ht="12.5">
       <c r="A70" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -2863,7 +2866,7 @@
     </row>
     <row r="71" spans="1:4" ht="12.5">
       <c r="A71" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -2871,7 +2874,7 @@
     </row>
     <row r="72" spans="1:4" ht="12.5">
       <c r="A72" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -2879,7 +2882,7 @@
     </row>
     <row r="73" spans="1:4" ht="12.5">
       <c r="A73" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -2887,7 +2890,7 @@
     </row>
     <row r="74" spans="1:4" ht="12.5">
       <c r="A74" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -2895,7 +2898,7 @@
     </row>
     <row r="75" spans="1:4" ht="12.5">
       <c r="A75" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B75" s="2"/>
       <c r="C75" s="2"/>
@@ -2903,7 +2906,7 @@
     </row>
     <row r="76" spans="1:4" ht="12.5">
       <c r="A76" s="2" t="s">
-        <v>238</v>
+        <v>138</v>
       </c>
       <c r="B76" s="2"/>
       <c r="C76" s="2"/>
@@ -2911,7 +2914,7 @@
     </row>
     <row r="77" spans="1:4" ht="12.5">
       <c r="A77" s="2" t="s">
-        <v>142</v>
+        <v>239</v>
       </c>
       <c r="B77" s="2"/>
       <c r="C77" s="2"/>
@@ -2919,7 +2922,7 @@
     </row>
     <row r="78" spans="1:4" ht="12.5">
       <c r="A78" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B78" s="2"/>
       <c r="C78" s="2"/>
@@ -2927,7 +2930,7 @@
     </row>
     <row r="79" spans="1:4" ht="12.5">
       <c r="A79" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B79" s="2"/>
       <c r="C79" s="2"/>
@@ -2935,7 +2938,7 @@
     </row>
     <row r="80" spans="1:4" ht="12.5">
       <c r="A80" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B80" s="2"/>
       <c r="C80" s="2"/>
@@ -2943,7 +2946,7 @@
     </row>
     <row r="81" spans="1:4" ht="12.5">
       <c r="A81" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B81" s="2"/>
       <c r="C81" s="2"/>
@@ -2951,7 +2954,7 @@
     </row>
     <row r="82" spans="1:4" ht="12.5">
       <c r="A82" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B82" s="2"/>
       <c r="C82" s="2"/>
@@ -2959,7 +2962,7 @@
     </row>
     <row r="83" spans="1:4" ht="12.5">
       <c r="A83" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" s="2"/>
@@ -2967,7 +2970,7 @@
     </row>
     <row r="84" spans="1:4" ht="12.5">
       <c r="A84" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" s="2"/>
@@ -2975,7 +2978,7 @@
     </row>
     <row r="85" spans="1:4" ht="12.5">
       <c r="A85" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" s="2"/>
@@ -2983,7 +2986,7 @@
     </row>
     <row r="86" spans="1:4" ht="12.5">
       <c r="A86" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" s="2"/>
@@ -2991,7 +2994,7 @@
     </row>
     <row r="87" spans="1:4" ht="12.5">
       <c r="A87" s="2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" s="2"/>
@@ -2999,7 +3002,7 @@
     </row>
     <row r="88" spans="1:4" ht="12.5">
       <c r="A88" s="2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" s="2"/>
@@ -3007,7 +3010,7 @@
     </row>
     <row r="89" spans="1:4" ht="12.5">
       <c r="A89" s="2" t="s">
-        <v>239</v>
+        <v>164</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" s="2"/>
@@ -3015,7 +3018,7 @@
     </row>
     <row r="90" spans="1:4" ht="12.5">
       <c r="A90" s="2" t="s">
-        <v>235</v>
+        <v>240</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" s="2"/>
@@ -3023,19 +3026,30 @@
     </row>
     <row r="91" spans="1:4" ht="12.5">
       <c r="A91" s="2" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
     <row r="92" spans="1:4" ht="12.5">
-      <c r="A92" s="2"/>
+      <c r="A92" s="2" t="s">
+        <v>241</v>
+      </c>
       <c r="B92" s="2"/>
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
     </row>
+    <row r="93" spans="1:4" ht="12.5">
+      <c r="A93" s="2"/>
+      <c r="B93" s="2"/>
+      <c r="C93" s="2"/>
+      <c r="D93" s="2"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3058,32 +3072,32 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15" customHeight="1">
       <c r="A2" s="9" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15" customHeight="1">
       <c r="A3" s="9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15" customHeight="1">
       <c r="A4" s="9" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15" customHeight="1">
       <c r="A5" s="9" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15" customHeight="1">
       <c r="A6" s="9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15" customHeight="1">
@@ -3118,12 +3132,12 @@
     </row>
     <row r="13" spans="1:1" ht="15" customHeight="1">
       <c r="A13" s="9" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15" customHeight="1">
       <c r="A14" s="9" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>